<commit_message>
se pueden asociar localizaciones a muestras con el excel, e iniciada la generación del excel de errores
</commit_message>
<xml_diff>
--- a/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
+++ b/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthem\Desktop\programas python\datos_prueba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthem\Desktop\programas_python\datos_prueba\datos_prueba\globalstaticfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68E04E47-8D7B-475C-BB09-F09E3EE2F089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B80D01-C78B-4D82-BF37-FDC122341A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="720" windowWidth="14355" windowHeight="15480" xr2:uid="{16C911DF-861F-4518-B37A-B68EA5D4CCB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16C911DF-861F-4518-B37A-B68EA5D4CCB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID Individuo</t>
   </si>
@@ -82,13 +82,34 @@
   </si>
   <si>
     <t>Lugar Procedencia</t>
+  </si>
+  <si>
+    <t>Congelador</t>
+  </si>
+  <si>
+    <t>Estante</t>
+  </si>
+  <si>
+    <t>Posición del rack en el estante</t>
+  </si>
+  <si>
+    <t>Rack</t>
+  </si>
+  <si>
+    <t>Posición de la caja en el rack</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Subposición</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +121,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,9 +154,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,19 +472,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1CF1C-662F-4A93-86E0-0B20BC98CAEA}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -495,9 +525,31 @@
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añadida la generación de un excel con los errores de subida
</commit_message>
<xml_diff>
--- a/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
+++ b/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthem\Desktop\programas_python\datos_prueba\datos_prueba\globalstaticfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B80D01-C78B-4D82-BF37-FDC122341A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA036FB-BA85-41D2-B0F9-BDE0EE6EE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16C911DF-861F-4518-B37A-B68EA5D4CCB1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ID Individuo</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Subposición</t>
+  </si>
+  <si>
+    <t>Estado actual</t>
   </si>
 </sst>
 </file>
@@ -472,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1CF1C-662F-4A93-86E0-0B20BC98CAEA}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,25 +529,28 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se pueden asociar muestras a un estudio desde el excel
</commit_message>
<xml_diff>
--- a/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
+++ b/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthem\Desktop\programas_python\datos_prueba\datos_prueba\globalstaticfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA036FB-BA85-41D2-B0F9-BDE0EE6EE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A12DB-2BCC-4013-A0E7-CA3174E4434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16C911DF-861F-4518-B37A-B68EA5D4CCB1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID Individuo</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>Estado actual</t>
+  </si>
+  <si>
+    <t>Estudio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +135,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,10 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,15 +486,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1CF1C-662F-4A93-86E0-0B20BC98CAEA}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -552,6 +563,9 @@
       </c>
       <c r="W1" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en la descarga del excel de muestras
</commit_message>
<xml_diff>
--- a/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
+++ b/datos_prueba/globalstaticfiles/Plantilla_muestras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthem\Desktop\programas_python\datos_prueba\datos_prueba\globalstaticfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A12DB-2BCC-4013-A0E7-CA3174E4434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B81034-5D95-400E-A95F-EAACCF5241AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16C911DF-861F-4518-B37A-B68EA5D4CCB1}"/>
   </bookViews>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1CF1C-662F-4A93-86E0-0B20BC98CAEA}">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>